<commit_message>
BackEndLog Table; EmployeeAuthority SP for Login; 資料層製作(未完);
</commit_message>
<xml_diff>
--- a/Documents/3.系統設計(Design_Phase)/EmployeeAuthority.xlsx
+++ b/Documents/3.系統設計(Design_Phase)/EmployeeAuthority.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$145</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$158</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="223">
   <si>
     <t>表格名稱：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -788,6 +788,122 @@
   </si>
   <si>
     <t>identity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表格名稱：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dbo.BackEndLog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>後端操作記錄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>序號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鍵值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中文名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英文名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>型別</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>允許Null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>說明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>流水號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seqno</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>帳號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EmpAccount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nvarchar(4000)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>作業時間</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OpDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外鍵值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>索引</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IX_BackEndLog_OpDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OpDate, include(EmpAccount, IP)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -951,7 +1067,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -977,21 +1093,10 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1003,7 +1108,21 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1300,9 +1419,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:G142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D126" sqref="D126:F126"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -1320,34 +1441,34 @@
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1"/>
     <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
       <c r="E3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="G3" s="19"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="8" t="s">
@@ -1502,23 +1623,23 @@
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7">
@@ -1526,20 +1647,20 @@
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12"/>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="1:7" ht="16.5">
       <c r="A16" s="1"/>
@@ -1548,8 +1669,8 @@
       <c r="D16" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
       <c r="G16" s="3" t="s">
         <v>186</v>
       </c>
@@ -1558,18 +1679,18 @@
       <c r="A18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
       <c r="E18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="19" t="s">
+      <c r="F18" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="G18" s="19"/>
+      <c r="G18" s="16"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="8" t="s">
@@ -1741,23 +1862,23 @@
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="3"/>
       <c r="D29" s="10"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="17"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="12"/>
       <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7">
@@ -1765,20 +1886,20 @@
       <c r="B30" s="2"/>
       <c r="C30" s="3"/>
       <c r="D30" s="10"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="17"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="12"/>
       <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="1:7" ht="16.5">
       <c r="A32" s="1"/>
@@ -1787,8 +1908,8 @@
       <c r="D32" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="E32" s="11"/>
-      <c r="F32" s="12"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="15"/>
       <c r="G32" s="3" t="s">
         <v>188</v>
       </c>
@@ -1797,18 +1918,18 @@
       <c r="A34" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
       <c r="E34" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F34" s="19" t="s">
+      <c r="F34" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G34" s="19"/>
+      <c r="G34" s="16"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="8" t="s">
@@ -2251,15 +2372,15 @@
       <c r="G58" s="3"/>
     </row>
     <row r="59" spans="1:7">
-      <c r="A59" s="18" t="s">
+      <c r="A59" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="18"/>
-      <c r="C59" s="18"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="18"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="1"/>
@@ -2268,8 +2389,8 @@
       <c r="D60" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="E60" s="16"/>
-      <c r="F60" s="17"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="12"/>
       <c r="G60" s="3"/>
     </row>
     <row r="61" spans="1:7">
@@ -2279,8 +2400,8 @@
       <c r="D61" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E61" s="16"/>
-      <c r="F61" s="17"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="12"/>
       <c r="G61" s="3"/>
     </row>
     <row r="62" spans="1:7">
@@ -2288,20 +2409,20 @@
       <c r="B62" s="2"/>
       <c r="C62" s="3"/>
       <c r="D62" s="10"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="17"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="12"/>
       <c r="G62" s="3"/>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="18" t="s">
+      <c r="A63" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="18"/>
-      <c r="G63" s="18"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
     </row>
     <row r="64" spans="1:7" ht="16.5">
       <c r="A64" s="1"/>
@@ -2310,8 +2431,8 @@
       <c r="D64" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="E64" s="11"/>
-      <c r="F64" s="12"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="15"/>
       <c r="G64" s="3" t="s">
         <v>119</v>
       </c>
@@ -2320,18 +2441,18 @@
       <c r="A66" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B66" s="19" t="s">
+      <c r="B66" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="C66" s="19"/>
-      <c r="D66" s="19"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="16"/>
       <c r="E66" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F66" s="19" t="s">
+      <c r="F66" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="G66" s="19"/>
+      <c r="G66" s="16"/>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="8" t="s">
@@ -2592,23 +2713,23 @@
       <c r="G80" s="3"/>
     </row>
     <row r="81" spans="1:7">
-      <c r="A81" s="18" t="s">
+      <c r="A81" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="B81" s="18"/>
-      <c r="C81" s="18"/>
-      <c r="D81" s="18"/>
-      <c r="E81" s="18"/>
-      <c r="F81" s="18"/>
-      <c r="G81" s="18"/>
+      <c r="B81" s="13"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="C82" s="3"/>
       <c r="D82" s="10"/>
-      <c r="E82" s="16"/>
-      <c r="F82" s="17"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="12"/>
       <c r="G82" s="3"/>
     </row>
     <row r="83" spans="1:7">
@@ -2616,20 +2737,20 @@
       <c r="B83" s="2"/>
       <c r="C83" s="3"/>
       <c r="D83" s="10"/>
-      <c r="E83" s="16"/>
-      <c r="F83" s="17"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="12"/>
       <c r="G83" s="3"/>
     </row>
     <row r="84" spans="1:7">
-      <c r="A84" s="18" t="s">
+      <c r="A84" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="B84" s="18"/>
-      <c r="C84" s="18"/>
-      <c r="D84" s="18"/>
-      <c r="E84" s="18"/>
-      <c r="F84" s="18"/>
-      <c r="G84" s="18"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
     </row>
     <row r="85" spans="1:7" ht="16.5">
       <c r="A85" s="1"/>
@@ -2638,8 +2759,8 @@
       <c r="D85" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="E85" s="11"/>
-      <c r="F85" s="12"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="15"/>
       <c r="G85" s="3" t="s">
         <v>190</v>
       </c>
@@ -2651,8 +2772,8 @@
       <c r="D86" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="E86" s="11"/>
-      <c r="F86" s="12"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="15"/>
       <c r="G86" s="3" t="s">
         <v>192</v>
       </c>
@@ -2661,18 +2782,18 @@
       <c r="A88" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B88" s="19" t="s">
+      <c r="B88" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="C88" s="19"/>
-      <c r="D88" s="19"/>
+      <c r="C88" s="16"/>
+      <c r="D88" s="16"/>
       <c r="E88" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F88" s="19" t="s">
+      <c r="F88" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="G88" s="19"/>
+      <c r="G88" s="16"/>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" s="8" t="s">
@@ -3060,15 +3181,15 @@
       <c r="G107" s="3"/>
     </row>
     <row r="108" spans="1:7">
-      <c r="A108" s="18" t="s">
+      <c r="A108" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="B108" s="18"/>
-      <c r="C108" s="18"/>
-      <c r="D108" s="18"/>
-      <c r="E108" s="18"/>
-      <c r="F108" s="18"/>
-      <c r="G108" s="18"/>
+      <c r="B108" s="13"/>
+      <c r="C108" s="13"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="13"/>
+      <c r="F108" s="13"/>
+      <c r="G108" s="13"/>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" s="1"/>
@@ -3077,8 +3198,8 @@
       <c r="D109" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="E109" s="16"/>
-      <c r="F109" s="17"/>
+      <c r="E109" s="11"/>
+      <c r="F109" s="12"/>
       <c r="G109" s="3"/>
     </row>
     <row r="110" spans="1:7">
@@ -3088,8 +3209,8 @@
       <c r="D110" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="E110" s="16"/>
-      <c r="F110" s="17"/>
+      <c r="E110" s="11"/>
+      <c r="F110" s="12"/>
       <c r="G110" s="3"/>
     </row>
     <row r="111" spans="1:7">
@@ -3097,64 +3218,68 @@
       <c r="B111" s="2"/>
       <c r="C111" s="3"/>
       <c r="D111" s="10"/>
-      <c r="E111" s="16"/>
-      <c r="F111" s="17"/>
+      <c r="E111" s="11"/>
+      <c r="F111" s="12"/>
       <c r="G111" s="3"/>
     </row>
     <row r="112" spans="1:7">
-      <c r="A112" s="18" t="s">
+      <c r="A112" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="B112" s="18"/>
-      <c r="C112" s="18"/>
-      <c r="D112" s="18"/>
-      <c r="E112" s="18"/>
-      <c r="F112" s="18"/>
-      <c r="G112" s="18"/>
+      <c r="B112" s="13"/>
+      <c r="C112" s="13"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="13"/>
+      <c r="F112" s="13"/>
+      <c r="G112" s="13"/>
     </row>
     <row r="113" spans="1:7" ht="16.5">
       <c r="A113" s="1"/>
       <c r="B113" s="2"/>
       <c r="C113" s="3"/>
       <c r="D113" s="10"/>
-      <c r="E113" s="11"/>
-      <c r="F113" s="12"/>
+      <c r="E113" s="14"/>
+      <c r="F113" s="15"/>
       <c r="G113" s="3"/>
     </row>
     <row r="115" spans="1:7">
       <c r="A115" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B115" s="13"/>
-      <c r="C115" s="14"/>
-      <c r="D115" s="15"/>
+        <v>194</v>
+      </c>
+      <c r="B115" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="C115" s="16"/>
+      <c r="D115" s="16"/>
       <c r="E115" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F115" s="13"/>
-      <c r="G115" s="15"/>
+        <v>17</v>
+      </c>
+      <c r="F115" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="G115" s="16"/>
     </row>
     <row r="116" spans="1:7">
-      <c r="A116" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B116" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C116" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D116" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E116" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F116" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G116" s="6" t="s">
-        <v>7</v>
+      <c r="A116" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B116" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C116" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="D116" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E116" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F116" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="G116" s="9" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -3162,22 +3287,38 @@
         <v>1</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C117" s="3"/>
-      <c r="D117" s="3"/>
-      <c r="E117" s="3"/>
-      <c r="F117" s="3"/>
-      <c r="G117" s="3"/>
+        <v>204</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="118" spans="1:7">
       <c r="A118" s="1">
         <v>2</v>
       </c>
       <c r="B118" s="2"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
-      <c r="E118" s="3"/>
+      <c r="C118" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>210</v>
+      </c>
       <c r="F118" s="3"/>
       <c r="G118" s="3"/>
     </row>
@@ -3186,9 +3327,15 @@
         <v>3</v>
       </c>
       <c r="B119" s="2"/>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
-      <c r="E119" s="3"/>
+      <c r="C119" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>212</v>
+      </c>
       <c r="F119" s="3"/>
       <c r="G119" s="3"/>
     </row>
@@ -3197,9 +3344,15 @@
         <v>4</v>
       </c>
       <c r="B120" s="2"/>
-      <c r="C120" s="3"/>
-      <c r="D120" s="3"/>
-      <c r="E120" s="3"/>
+      <c r="C120" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>215</v>
+      </c>
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
     </row>
@@ -3208,136 +3361,264 @@
         <v>5</v>
       </c>
       <c r="B121" s="2"/>
-      <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
-      <c r="E121" s="3"/>
+      <c r="C121" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>218</v>
+      </c>
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
     </row>
     <row r="122" spans="1:7">
-      <c r="A122" s="1">
-        <v>6</v>
-      </c>
-      <c r="B122" s="2"/>
-      <c r="C122" s="3"/>
-      <c r="D122" s="3"/>
-      <c r="E122" s="3"/>
-      <c r="F122" s="3"/>
-      <c r="G122" s="3"/>
+      <c r="A122" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="B122" s="13"/>
+      <c r="C122" s="13"/>
+      <c r="D122" s="13"/>
+      <c r="E122" s="13"/>
+      <c r="F122" s="13"/>
+      <c r="G122" s="13"/>
     </row>
     <row r="123" spans="1:7">
-      <c r="A123" s="1">
-        <v>7</v>
-      </c>
+      <c r="A123" s="1"/>
       <c r="B123" s="2"/>
       <c r="C123" s="3"/>
-      <c r="D123" s="3"/>
-      <c r="E123" s="3"/>
-      <c r="F123" s="3"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="11"/>
+      <c r="F123" s="12"/>
       <c r="G123" s="3"/>
     </row>
     <row r="124" spans="1:7">
-      <c r="A124" s="1">
-        <v>8</v>
-      </c>
+      <c r="A124" s="1"/>
       <c r="B124" s="2"/>
       <c r="C124" s="3"/>
-      <c r="D124" s="3"/>
-      <c r="E124" s="3"/>
-      <c r="F124" s="3"/>
+      <c r="D124" s="10"/>
+      <c r="E124" s="11"/>
+      <c r="F124" s="12"/>
       <c r="G124" s="3"/>
     </row>
     <row r="125" spans="1:7">
-      <c r="A125" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B125" s="18"/>
-      <c r="C125" s="18"/>
-      <c r="D125" s="18"/>
-      <c r="E125" s="18"/>
-      <c r="F125" s="18"/>
-      <c r="G125" s="18"/>
-    </row>
-    <row r="126" spans="1:7">
+      <c r="A125" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B125" s="13"/>
+      <c r="C125" s="13"/>
+      <c r="D125" s="13"/>
+      <c r="E125" s="13"/>
+      <c r="F125" s="13"/>
+      <c r="G125" s="13"/>
+    </row>
+    <row r="126" spans="1:7" ht="16.5">
       <c r="A126" s="1"/>
       <c r="B126" s="2"/>
       <c r="C126" s="3"/>
-      <c r="D126" s="10"/>
-      <c r="E126" s="16"/>
-      <c r="F126" s="17"/>
-      <c r="G126" s="3"/>
-    </row>
-    <row r="127" spans="1:7">
-      <c r="A127" s="1"/>
-      <c r="B127" s="2"/>
-      <c r="C127" s="3"/>
-      <c r="D127" s="10"/>
-      <c r="E127" s="16"/>
-      <c r="F127" s="17"/>
-      <c r="G127" s="3"/>
+      <c r="D126" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="E126" s="14"/>
+      <c r="F126" s="15"/>
+      <c r="G126" s="3" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="128" spans="1:7">
-      <c r="A128" s="18" t="s">
+      <c r="A128" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B128" s="18"/>
+      <c r="C128" s="19"/>
+      <c r="D128" s="20"/>
+      <c r="E128" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F128" s="18"/>
+      <c r="G128" s="20"/>
+    </row>
+    <row r="129" spans="1:7">
+      <c r="A129" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C129" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D129" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E129" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F129" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G129" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
+      <c r="A130" s="1">
+        <v>1</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C130" s="3"/>
+      <c r="D130" s="3"/>
+      <c r="E130" s="3"/>
+      <c r="F130" s="3"/>
+      <c r="G130" s="3"/>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="A131" s="1">
+        <v>2</v>
+      </c>
+      <c r="B131" s="2"/>
+      <c r="C131" s="3"/>
+      <c r="D131" s="3"/>
+      <c r="E131" s="3"/>
+      <c r="F131" s="3"/>
+      <c r="G131" s="3"/>
+    </row>
+    <row r="132" spans="1:7">
+      <c r="A132" s="1">
+        <v>3</v>
+      </c>
+      <c r="B132" s="2"/>
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="3"/>
+      <c r="G132" s="3"/>
+    </row>
+    <row r="133" spans="1:7">
+      <c r="A133" s="1">
+        <v>4</v>
+      </c>
+      <c r="B133" s="2"/>
+      <c r="C133" s="3"/>
+      <c r="D133" s="3"/>
+      <c r="E133" s="3"/>
+      <c r="F133" s="3"/>
+      <c r="G133" s="3"/>
+    </row>
+    <row r="134" spans="1:7">
+      <c r="A134" s="1">
+        <v>5</v>
+      </c>
+      <c r="B134" s="2"/>
+      <c r="C134" s="3"/>
+      <c r="D134" s="3"/>
+      <c r="E134" s="3"/>
+      <c r="F134" s="3"/>
+      <c r="G134" s="3"/>
+    </row>
+    <row r="135" spans="1:7">
+      <c r="A135" s="1">
+        <v>6</v>
+      </c>
+      <c r="B135" s="2"/>
+      <c r="C135" s="3"/>
+      <c r="D135" s="3"/>
+      <c r="E135" s="3"/>
+      <c r="F135" s="3"/>
+      <c r="G135" s="3"/>
+    </row>
+    <row r="136" spans="1:7">
+      <c r="A136" s="1">
+        <v>7</v>
+      </c>
+      <c r="B136" s="2"/>
+      <c r="C136" s="3"/>
+      <c r="D136" s="3"/>
+      <c r="E136" s="3"/>
+      <c r="F136" s="3"/>
+      <c r="G136" s="3"/>
+    </row>
+    <row r="137" spans="1:7">
+      <c r="A137" s="1">
+        <v>8</v>
+      </c>
+      <c r="B137" s="2"/>
+      <c r="C137" s="3"/>
+      <c r="D137" s="3"/>
+      <c r="E137" s="3"/>
+      <c r="F137" s="3"/>
+      <c r="G137" s="3"/>
+    </row>
+    <row r="138" spans="1:7">
+      <c r="A138" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B138" s="13"/>
+      <c r="C138" s="13"/>
+      <c r="D138" s="13"/>
+      <c r="E138" s="13"/>
+      <c r="F138" s="13"/>
+      <c r="G138" s="13"/>
+    </row>
+    <row r="139" spans="1:7">
+      <c r="A139" s="1"/>
+      <c r="B139" s="2"/>
+      <c r="C139" s="3"/>
+      <c r="D139" s="10"/>
+      <c r="E139" s="11"/>
+      <c r="F139" s="12"/>
+      <c r="G139" s="3"/>
+    </row>
+    <row r="140" spans="1:7">
+      <c r="A140" s="1"/>
+      <c r="B140" s="2"/>
+      <c r="C140" s="3"/>
+      <c r="D140" s="10"/>
+      <c r="E140" s="11"/>
+      <c r="F140" s="12"/>
+      <c r="G140" s="3"/>
+    </row>
+    <row r="141" spans="1:7">
+      <c r="A141" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B128" s="18"/>
-      <c r="C128" s="18"/>
-      <c r="D128" s="18"/>
-      <c r="E128" s="18"/>
-      <c r="F128" s="18"/>
-      <c r="G128" s="18"/>
-    </row>
-    <row r="129" spans="1:7" ht="16.5">
-      <c r="A129" s="1"/>
-      <c r="B129" s="2"/>
-      <c r="C129" s="3"/>
-      <c r="D129" s="10"/>
-      <c r="E129" s="11"/>
-      <c r="F129" s="12"/>
-      <c r="G129" s="3"/>
+      <c r="B141" s="13"/>
+      <c r="C141" s="13"/>
+      <c r="D141" s="13"/>
+      <c r="E141" s="13"/>
+      <c r="F141" s="13"/>
+      <c r="G141" s="13"/>
+    </row>
+    <row r="142" spans="1:7" ht="16.5">
+      <c r="A142" s="1"/>
+      <c r="B142" s="2"/>
+      <c r="C142" s="3"/>
+      <c r="D142" s="10"/>
+      <c r="E142" s="14"/>
+      <c r="F142" s="15"/>
+      <c r="G142" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="47">
-    <mergeCell ref="D109:F109"/>
-    <mergeCell ref="D110:F110"/>
-    <mergeCell ref="D111:F111"/>
-    <mergeCell ref="A112:G112"/>
-    <mergeCell ref="D113:F113"/>
-    <mergeCell ref="A84:G84"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="A108:G108"/>
-    <mergeCell ref="D86:F86"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="A81:G81"/>
-    <mergeCell ref="D82:F82"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="D13:F13"/>
+  <mergeCells count="54">
+    <mergeCell ref="A125:G125"/>
+    <mergeCell ref="D126:F126"/>
+    <mergeCell ref="B115:D115"/>
+    <mergeCell ref="F115:G115"/>
+    <mergeCell ref="A122:G122"/>
+    <mergeCell ref="D123:F123"/>
+    <mergeCell ref="D124:F124"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="D129:F129"/>
-    <mergeCell ref="B115:D115"/>
-    <mergeCell ref="F115:G115"/>
-    <mergeCell ref="D127:F127"/>
-    <mergeCell ref="A125:G125"/>
-    <mergeCell ref="D126:F126"/>
-    <mergeCell ref="A128:G128"/>
+    <mergeCell ref="D142:F142"/>
+    <mergeCell ref="B128:D128"/>
+    <mergeCell ref="F128:G128"/>
+    <mergeCell ref="D140:F140"/>
+    <mergeCell ref="A138:G138"/>
+    <mergeCell ref="D139:F139"/>
+    <mergeCell ref="A141:G141"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="A59:G59"/>
@@ -3345,6 +3626,37 @@
     <mergeCell ref="D61:F61"/>
     <mergeCell ref="D62:F62"/>
     <mergeCell ref="A63:G63"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="A81:G81"/>
+    <mergeCell ref="D82:F82"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="A84:G84"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="A108:G108"/>
+    <mergeCell ref="D86:F86"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="D109:F109"/>
+    <mergeCell ref="D110:F110"/>
+    <mergeCell ref="D111:F111"/>
+    <mergeCell ref="A112:G112"/>
+    <mergeCell ref="D113:F113"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>